<commit_message>
update answer_processing scripts, add bonuse output, whether to reject/accept
</commit_message>
<xml_diff>
--- a/Scripts/tmp.xlsx
+++ b/Scripts/tmp.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="B1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -374,62 +374,47 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>accepted_and_use</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>all_audio_played</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>assignment</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>correct_cmps</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>correct_gold_question</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>correct_math</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>correct_tps</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>variance_in_ratings</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>worker_id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>35GCEFQ6I93Y3FGGY5K5J6ETKDRZ3V</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>4</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>ARAF31KCGJ5AA</t>
         </is>
       </c>
     </row>

</xml_diff>